<commit_message>
oll's alg pairer works
</commit_message>
<xml_diff>
--- a/Solver/examples/exampleCubeFileModel.xlsx
+++ b/Solver/examples/exampleCubeFileModel.xlsx
@@ -17,6 +17,14 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+  <si>
+    <t xml:space="preserve">OLL</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -55,7 +63,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -96,6 +104,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFFFF"/>
         <bgColor rgb="FFFFFFCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFDDDDDD"/>
+        <bgColor rgb="FFCCFFCC"/>
       </patternFill>
     </fill>
   </fills>
@@ -140,7 +154,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="11">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -170,6 +184,18 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="4" fillId="7" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="8" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="8" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -207,7 +233,7 @@
       <rgbColor rgb="FF660066"/>
       <rgbColor rgb="FFFF8080"/>
       <rgbColor rgb="FF0066CC"/>
-      <rgbColor rgb="FFCCCCFF"/>
+      <rgbColor rgb="FFDDDDDD"/>
       <rgbColor rgb="FF000080"/>
       <rgbColor rgb="FFFF00FF"/>
       <rgbColor rgb="FFFFFF00"/>
@@ -250,18 +276,18 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:O9"/>
+  <dimension ref="A1:O15"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="T8" activeCellId="0" sqref="T8"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J11" activeCellId="0" sqref="J11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.34375" defaultRowHeight="35.05" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.34375" defaultRowHeight="38.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="1" style="1" width="8.33"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="35.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="38.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="n">
         <v>2</v>
       </c>
@@ -275,7 +301,7 @@
       <c r="E1" s="0"/>
       <c r="F1" s="0"/>
     </row>
-    <row r="2" customFormat="false" ht="35.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="38.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="n">
         <v>9</v>
       </c>
@@ -289,7 +315,7 @@
       <c r="E2" s="0"/>
       <c r="F2" s="0"/>
     </row>
-    <row r="3" customFormat="false" ht="35.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="38.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="n">
         <v>8</v>
       </c>
@@ -303,7 +329,7 @@
       <c r="E3" s="0"/>
       <c r="F3" s="0"/>
     </row>
-    <row r="4" customFormat="false" ht="35.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="38.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="n">
         <f aca="false">A1+9</f>
         <v>11</v>
@@ -353,7 +379,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="35.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="38.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="n">
         <f aca="false">A2+9</f>
         <v>18</v>
@@ -403,7 +429,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="35.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="38.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="n">
         <f aca="false">A3+9</f>
         <v>17</v>
@@ -453,7 +479,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="35.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="38.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D7" s="0"/>
       <c r="E7" s="0"/>
       <c r="F7" s="0"/>
@@ -473,7 +499,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="35.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="38.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D8" s="0"/>
       <c r="E8" s="0"/>
       <c r="F8" s="0"/>
@@ -493,7 +519,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="35.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="38.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D9" s="0"/>
       <c r="E9" s="0"/>
       <c r="F9" s="0"/>
@@ -512,6 +538,160 @@
         <f aca="false">L6+9</f>
         <v>51</v>
       </c>
+    </row>
+    <row r="10" customFormat="false" ht="38.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="J10" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="38.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0"/>
+      <c r="B11" s="8"/>
+      <c r="C11" s="9" t="n">
+        <v>1</v>
+      </c>
+      <c r="D11" s="9" t="n">
+        <v>2</v>
+      </c>
+      <c r="E11" s="9" t="n">
+        <v>3</v>
+      </c>
+      <c r="F11" s="8"/>
+      <c r="H11" s="10"/>
+      <c r="I11" s="2" t="n">
+        <v>18</v>
+      </c>
+      <c r="J11" s="2" t="n">
+        <v>17</v>
+      </c>
+      <c r="K11" s="2" t="n">
+        <v>16</v>
+      </c>
+      <c r="L11" s="10"/>
+    </row>
+    <row r="12" customFormat="false" ht="38.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0"/>
+      <c r="B12" s="9" t="n">
+        <v>4</v>
+      </c>
+      <c r="C12" s="9" t="n">
+        <v>5</v>
+      </c>
+      <c r="D12" s="9" t="n">
+        <v>6</v>
+      </c>
+      <c r="E12" s="9" t="n">
+        <v>7</v>
+      </c>
+      <c r="F12" s="9" t="n">
+        <v>8</v>
+      </c>
+      <c r="H12" s="2" t="n">
+        <v>19</v>
+      </c>
+      <c r="I12" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="J12" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="K12" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="L12" s="2" t="n">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="38.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0"/>
+      <c r="B13" s="9" t="n">
+        <v>9</v>
+      </c>
+      <c r="C13" s="9" t="n">
+        <v>10</v>
+      </c>
+      <c r="D13" s="9" t="n">
+        <v>11</v>
+      </c>
+      <c r="E13" s="9" t="n">
+        <v>12</v>
+      </c>
+      <c r="F13" s="9" t="n">
+        <v>13</v>
+      </c>
+      <c r="H13" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="I13" s="2" t="n">
+        <v>9</v>
+      </c>
+      <c r="J13" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="K13" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="L13" s="2" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="38.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0"/>
+      <c r="B14" s="9" t="n">
+        <v>14</v>
+      </c>
+      <c r="C14" s="9" t="n">
+        <v>15</v>
+      </c>
+      <c r="D14" s="9" t="n">
+        <v>16</v>
+      </c>
+      <c r="E14" s="9" t="n">
+        <v>17</v>
+      </c>
+      <c r="F14" s="9" t="n">
+        <v>18</v>
+      </c>
+      <c r="H14" s="2" t="n">
+        <v>21</v>
+      </c>
+      <c r="I14" s="2" t="n">
+        <v>8</v>
+      </c>
+      <c r="J14" s="2" t="n">
+        <v>7</v>
+      </c>
+      <c r="K14" s="2" t="n">
+        <v>6</v>
+      </c>
+      <c r="L14" s="2" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="38.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0"/>
+      <c r="B15" s="8"/>
+      <c r="C15" s="9" t="n">
+        <v>19</v>
+      </c>
+      <c r="D15" s="9" t="n">
+        <v>20</v>
+      </c>
+      <c r="E15" s="9" t="n">
+        <v>21</v>
+      </c>
+      <c r="F15" s="8"/>
+      <c r="H15" s="10"/>
+      <c r="I15" s="2" t="n">
+        <v>10</v>
+      </c>
+      <c r="J15" s="2" t="n">
+        <v>11</v>
+      </c>
+      <c r="K15" s="2" t="n">
+        <v>12</v>
+      </c>
+      <c r="L15" s="10"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>